<commit_message>
Update Equipment Checklist December 2025.xlsx.xlsx
</commit_message>
<xml_diff>
--- a/Equipment Checklist December 2025.xlsx.xlsx
+++ b/Equipment Checklist December 2025.xlsx.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="510" yWindow="585" windowWidth="18855" windowHeight="7110"/>
+    <workbookView xWindow="510" yWindow="585" windowWidth="18855" windowHeight="7110" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Ingersoll" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="47">
   <si>
     <t>Date</t>
   </si>
@@ -177,6 +177,12 @@
   </si>
   <si>
     <t>Not in auto with Grid</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>Benjamin</t>
   </si>
 </sst>
 </file>
@@ -397,7 +403,73 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="21">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -790,8 +862,8 @@
   </sheetPr>
   <dimension ref="A1:R32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1025,12 +1097,22 @@
       <c r="Q6" s="8"/>
     </row>
     <row r="7" spans="1:18" ht="16.5">
-      <c r="A7" s="12"/>
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="18"/>
+      <c r="A7" s="12">
+        <v>45997</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7" s="18">
+        <v>11372</v>
+      </c>
       <c r="E7" s="18"/>
-      <c r="F7" s="8"/>
+      <c r="F7" s="8" t="s">
+        <v>42</v>
+      </c>
       <c r="G7" s="8"/>
       <c r="H7" s="8"/>
       <c r="I7" s="18"/>
@@ -1044,12 +1126,22 @@
       <c r="Q7" s="25"/>
     </row>
     <row r="8" spans="1:18" ht="16.5">
-      <c r="A8" s="12"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="18"/>
+      <c r="A8" s="12">
+        <v>45998</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="D8" s="18">
+        <v>11372</v>
+      </c>
       <c r="E8" s="18"/>
-      <c r="F8" s="8"/>
+      <c r="F8" s="8" t="s">
+        <v>42</v>
+      </c>
       <c r="G8" s="8"/>
       <c r="H8" s="8"/>
       <c r="I8" s="18"/>
@@ -1063,12 +1155,22 @@
       <c r="Q8" s="25"/>
     </row>
     <row r="9" spans="1:18" ht="16.5">
-      <c r="A9" s="12"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="18"/>
+      <c r="A9" s="12">
+        <v>45999</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="D9" s="18">
+        <v>11372</v>
+      </c>
       <c r="E9" s="18"/>
-      <c r="F9" s="8"/>
+      <c r="F9" s="8" t="s">
+        <v>42</v>
+      </c>
       <c r="G9" s="8"/>
       <c r="H9" s="8"/>
       <c r="I9" s="18"/>
@@ -1520,30 +1622,30 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="F33:P100 G2:I32 L2:P32">
-    <cfRule type="expression" dxfId="11" priority="22">
+    <cfRule type="expression" dxfId="20" priority="22">
       <formula>OR(LOWER(F2)="low",LOWER(F2)="y")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:K32">
-    <cfRule type="expression" dxfId="10" priority="12">
+    <cfRule type="expression" dxfId="19" priority="12">
       <formula>AND(K2&lt;&gt;"", OR(K2&lt;2, K2&gt;10))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L2:L32">
-    <cfRule type="expression" dxfId="9" priority="5">
+    <cfRule type="expression" dxfId="18" priority="5">
       <formula>AND(L2&lt;&gt;"", ISNUMBER(L2), L2&gt;=106, L2&lt;=120)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="6">
+    <cfRule type="expression" dxfId="17" priority="6">
       <formula>AND(L2&lt;&gt;" ", ISNUMBER(L2), L2&gt;=100, L2&lt;=105)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G32">
-    <cfRule type="expression" dxfId="7" priority="3">
+    <cfRule type="expression" dxfId="16" priority="3">
       <formula>AND(G2&lt;&gt;"", LOWER(G2)="yes")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:H32">
-    <cfRule type="expression" dxfId="6" priority="1">
+    <cfRule type="expression" dxfId="15" priority="1">
       <formula>AND(H2&lt;&gt;"", LOWER(H2)="yes")</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1560,7 +1662,7 @@
   <dimension ref="A1:R32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1888,60 +1990,150 @@
       <c r="Q6" s="22"/>
     </row>
     <row r="7" spans="1:18" ht="16.5">
-      <c r="A7" s="12"/>
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="18"/>
+      <c r="A7" s="12">
+        <v>45997</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7" s="18">
+        <v>13823</v>
+      </c>
       <c r="E7" s="18"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="8"/>
-      <c r="I7" s="8"/>
-      <c r="J7" s="9"/>
-      <c r="K7" s="9"/>
-      <c r="L7" s="8"/>
-      <c r="M7" s="8"/>
-      <c r="N7" s="8"/>
-      <c r="O7" s="8"/>
-      <c r="P7" s="8"/>
+      <c r="F7" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="H7" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="I7" s="8">
+        <v>7</v>
+      </c>
+      <c r="J7" s="9">
+        <v>62</v>
+      </c>
+      <c r="K7" s="9">
+        <v>20</v>
+      </c>
+      <c r="L7" s="8">
+        <v>72</v>
+      </c>
+      <c r="M7" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="N7" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="O7" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="P7" s="8" t="s">
+        <v>40</v>
+      </c>
       <c r="Q7" s="22"/>
     </row>
     <row r="8" spans="1:18" ht="16.5">
-      <c r="A8" s="12"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="18"/>
+      <c r="A8" s="12">
+        <v>45998</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="D8" s="18">
+        <v>13848</v>
+      </c>
       <c r="E8" s="18"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
-      <c r="I8" s="8"/>
-      <c r="J8" s="9"/>
-      <c r="K8" s="9"/>
-      <c r="L8" s="8"/>
-      <c r="M8" s="8"/>
-      <c r="N8" s="8"/>
-      <c r="O8" s="8"/>
-      <c r="P8" s="8"/>
+      <c r="F8" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="H8" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="I8" s="8">
+        <v>7</v>
+      </c>
+      <c r="J8" s="9">
+        <v>68</v>
+      </c>
+      <c r="K8" s="9">
+        <v>24</v>
+      </c>
+      <c r="L8" s="8">
+        <v>73</v>
+      </c>
+      <c r="M8" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="N8" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="O8" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="P8" s="8" t="s">
+        <v>40</v>
+      </c>
       <c r="Q8" s="8"/>
     </row>
     <row r="9" spans="1:18" ht="16.5">
-      <c r="A9" s="12"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="18"/>
+      <c r="A9" s="12">
+        <v>45999</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="D9" s="18">
+        <v>13872</v>
+      </c>
       <c r="E9" s="18"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="8"/>
-      <c r="J9" s="9"/>
-      <c r="K9" s="9"/>
-      <c r="L9" s="8"/>
-      <c r="M9" s="8"/>
-      <c r="N9" s="8"/>
-      <c r="O9" s="8"/>
-      <c r="P9" s="8"/>
+      <c r="F9" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="H9" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="I9" s="8">
+        <v>7</v>
+      </c>
+      <c r="J9" s="9">
+        <v>60</v>
+      </c>
+      <c r="K9" s="9">
+        <v>20</v>
+      </c>
+      <c r="L9" s="8">
+        <v>73</v>
+      </c>
+      <c r="M9" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="N9" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="O9" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="P9" s="8" t="s">
+        <v>40</v>
+      </c>
       <c r="Q9" s="8"/>
     </row>
     <row r="10" spans="1:18" ht="16.5">
@@ -2384,19 +2576,34 @@
       <c r="Q32" s="8"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="F33:P100 F2:I32 L2:P32">
-    <cfRule type="expression" dxfId="5" priority="3">
+  <conditionalFormatting sqref="F33:P100 F2:I6 L2:P6 L10:P32 F10:I32">
+    <cfRule type="expression" dxfId="14" priority="6">
       <formula>OR(LOWER(F2)="low",LOWER(F2)="y")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J32">
-    <cfRule type="expression" dxfId="4" priority="2">
+  <conditionalFormatting sqref="J2:J6 J10:J32">
+    <cfRule type="expression" dxfId="13" priority="5">
       <formula>AND(J2&lt;&gt;"", OR(J2&lt;3, J2&gt;8))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K2:K32">
-    <cfRule type="expression" dxfId="3" priority="1">
+  <conditionalFormatting sqref="K2:K6 K10:K32">
+    <cfRule type="expression" dxfId="12" priority="4">
       <formula>AND(K2&lt;&gt;"", OR(K2&lt;2, K2&gt;10))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F7:I9 L7:P9">
+    <cfRule type="expression" dxfId="5" priority="3">
+      <formula>OR(LOWER(F7)="low",LOWER(F7)="y")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J7:J9">
+    <cfRule type="expression" dxfId="3" priority="2">
+      <formula>AND(J7&lt;&gt;"", OR(J7&lt;3, J7&gt;8))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K7:K9">
+    <cfRule type="expression" dxfId="1" priority="1">
+      <formula>AND(K7&lt;&gt;"", OR(K7&lt;2, K7&gt;10))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2411,8 +2618,8 @@
   </sheetPr>
   <dimension ref="A1:P32"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="O7" sqref="O7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3071,7 +3278,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="J2:N100">
-    <cfRule type="expression" dxfId="2" priority="3">
+    <cfRule type="expression" dxfId="11" priority="3">
       <formula>OR(LOWER(J2)="low",LOWER(J2)="y")</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3128,10 +3335,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:E100">
-    <cfRule type="expression" dxfId="1" priority="1">
+    <cfRule type="expression" dxfId="10" priority="1">
       <formula>OR(LOWER(B2)="replace",LOWER(B2)="adjust",LOWER(B2)="n")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="2">
+    <cfRule type="expression" dxfId="9" priority="2">
       <formula>OR(LOWER(B2)="clean",LOWER(B2)="ok",LOWER(B2)="y")</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>